<commit_message>
fixed db to conform with test
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="165" windowWidth="28815" windowHeight="7125" tabRatio="539" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="165" windowWidth="28815" windowHeight="7125" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$AY$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$AY$16</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="76">
   <si>
     <t>Sr.No</t>
   </si>
@@ -71,9 +71,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>bad</t>
-  </si>
-  <si>
     <t>cc - cr2032</t>
   </si>
   <si>
@@ -83,57 +80,6 @@
     <t>Cell Name</t>
   </si>
   <si>
-    <t>20131021_es024_01_cc</t>
-  </si>
-  <si>
-    <t>20131021_es024_02_cc</t>
-  </si>
-  <si>
-    <t>20131021_es024_03_cc</t>
-  </si>
-  <si>
-    <t>20131021_es025_01_cc</t>
-  </si>
-  <si>
-    <t>20131021_es025_02_cc</t>
-  </si>
-  <si>
-    <t>20131021_es025_03_cc</t>
-  </si>
-  <si>
-    <t>20131021_es026_01_cc</t>
-  </si>
-  <si>
-    <t>20131021_es026_02_cc</t>
-  </si>
-  <si>
-    <t>20131025_es023_29_cc</t>
-  </si>
-  <si>
-    <t>20131025_es023_30_cc</t>
-  </si>
-  <si>
-    <t>20131025_es014_20_cc</t>
-  </si>
-  <si>
-    <t>20131029_es014_21_cc</t>
-  </si>
-  <si>
-    <t>20131029_es023_32_cc</t>
-  </si>
-  <si>
-    <t>20131029_es023_31_cc</t>
-  </si>
-  <si>
-    <t>20131029_es027_01_cc</t>
-  </si>
-  <si>
-    <t>20131029_es027_02_cc</t>
-  </si>
-  <si>
-    <t>20131029_es027_03_cc</t>
-  </si>
-  <si>
     <t>txt</t>
   </si>
   <si>
@@ -161,9 +107,6 @@
     <t>B02</t>
   </si>
   <si>
-    <t>Coin-cell tests</t>
-  </si>
-  <si>
     <t>Selected</t>
   </si>
   <si>
@@ -212,15 +155,6 @@
     <t>2_01</t>
   </si>
   <si>
-    <t>2_19</t>
-  </si>
-  <si>
-    <t>2_20</t>
-  </si>
-  <si>
-    <t>2_21</t>
-  </si>
-  <si>
     <t>2_22</t>
   </si>
   <si>
@@ -287,12 +221,6 @@
     <t>Project</t>
   </si>
   <si>
-    <t>cellpy</t>
-  </si>
-  <si>
-    <t>simple test</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -303,6 +231,24 @@
   </si>
   <si>
     <t>F5</t>
+  </si>
+  <si>
+    <t>exp001</t>
+  </si>
+  <si>
+    <t>20160805_test001_45_cc</t>
+  </si>
+  <si>
+    <t>20160805_test001_46_cc</t>
+  </si>
+  <si>
+    <t>20160805_test001_47_cc</t>
+  </si>
+  <si>
+    <t>exp002</t>
+  </si>
+  <si>
+    <t>test comment general</t>
   </si>
 </sst>
 </file>
@@ -310,8 +256,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -379,15 +325,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -753,13 +699,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AY19"/>
+  <dimension ref="A1:AY16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q25" sqref="Q25"/>
+      <selection pane="bottomRight" activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -814,97 +760,97 @@
         <v>14</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>58</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="17" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="AF1" s="5" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="AI1" s="6" t="s">
         <v>2</v>
@@ -937,10 +883,10 @@
         <v>10</v>
       </c>
       <c r="AW1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="AY1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:51" ht="15" x14ac:dyDescent="0.25">
@@ -951,115 +897,115 @@
         <v>15</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="X2" s="15" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AJ2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AN2" s="9" t="s">
         <v>4</v>
@@ -1074,45 +1020,49 @@
       <c r="AT2" s="11"/>
       <c r="AU2" s="11"/>
       <c r="AV2" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AX2" s="25"/>
     </row>
     <row r="3" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>177</v>
+        <v>614</v>
       </c>
       <c r="B3" s="6">
-        <v>15</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="21">
+        <v>1</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="21" t="s">
+        <v>66</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
-        <v>90</v>
+      <c r="J3" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="N3" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="O3" s="21" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="R3" s="5" t="str">
-        <f t="shared" ref="R3:R19" si="0">Q3</f>
-        <v>20131021_es024_01_cc</v>
+        <f t="shared" ref="R3:R16" si="0">Q3</f>
+        <v>20160805_test001_45_cc</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5">
@@ -1161,22 +1111,22 @@
         <v>0</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="AJ3" s="7">
-        <v>1.690042957132986</v>
+        <v>0.51026231569116942</v>
       </c>
       <c r="AK3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AN3" s="9">
-        <v>2.817499999999999</v>
+        <v>2.8174999999999999</v>
       </c>
       <c r="AO3" s="8"/>
       <c r="AP3" s="5"/>
@@ -1187,53 +1137,57 @@
       <c r="AS3" s="11"/>
       <c r="AT3" s="11"/>
       <c r="AU3" s="11"/>
-      <c r="AV3" s="5"/>
+      <c r="AV3" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="AX3" s="25"/>
     </row>
     <row r="4" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>178</v>
+        <v>615</v>
       </c>
       <c r="B4" s="6">
-        <v>15</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="21">
+        <v>1</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="21"/>
+      <c r="F4" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
-        <v>90</v>
+      <c r="J4" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="21" t="s">
-        <v>41</v>
+      <c r="O4" s="21">
+        <v>2</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="R4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es024_02_cc</v>
+        <v>20160805_test001_46_cc</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="19">
         <v>0</v>
@@ -1275,16 +1229,16 @@
         <v>0</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ4" s="7">
-        <v>1.5220883775421308</v>
+        <v>0.45438760079739932</v>
       </c>
       <c r="AK4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL4" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL4" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM4" s="5" t="s">
         <v>11</v>
@@ -1306,44 +1260,44 @@
     </row>
     <row r="5" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>179</v>
+        <v>616</v>
       </c>
       <c r="B5" s="6">
-        <v>15</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>89</v>
+        <v>45</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="21">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="21" t="s">
+        <v>66</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
-        <v>90</v>
+      <c r="J5" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="O5" s="21" t="s">
-        <v>41</v>
+      <c r="O5" s="21">
+        <v>2</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="5" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="R5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es024_03_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" s="5">
         <v>0</v>
@@ -1388,16 +1342,16 @@
         <v>0</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="AJ5" s="7">
-        <v>1.6180624230226202</v>
+        <v>0.495843034428261</v>
       </c>
       <c r="AK5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL5" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM5" s="5" t="s">
         <v>11</v>
@@ -1419,45 +1373,47 @@
     </row>
     <row r="6" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>180</v>
+        <v>617</v>
       </c>
       <c r="B6" s="6">
-        <v>15</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
-        <v>88</v>
+      <c r="J6" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="21" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="R6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_01_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="5">
         <v>0</v>
@@ -1502,16 +1458,16 @@
         <v>0</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="AJ6" s="7">
-        <v>1.7379435241867718</v>
+        <v>0.45438760079739932</v>
       </c>
       <c r="AK6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL6" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>11</v>
@@ -1533,43 +1489,45 @@
     </row>
     <row r="7" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>181</v>
+        <v>618</v>
       </c>
       <c r="B7" s="6">
-        <v>15</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="6" t="s">
-        <v>88</v>
+      <c r="J7" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="21" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="R7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_02_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="5">
         <v>0</v>
@@ -1614,16 +1572,16 @@
         <v>0</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="AJ7" s="7">
-        <v>1.6719646501020284</v>
+        <v>0.44717796016594541</v>
       </c>
       <c r="AK7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL7" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>11</v>
@@ -1645,43 +1603,45 @@
     </row>
     <row r="8" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>182</v>
+        <v>619</v>
       </c>
       <c r="B8" s="6">
-        <v>15</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="21">
+        <v>1</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="6" t="s">
-        <v>88</v>
+      <c r="J8" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="21" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="5" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="R8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_03_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="5">
         <v>0</v>
@@ -1726,16 +1686,16 @@
         <v>0</v>
       </c>
       <c r="AI8" s="6" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="AJ8" s="7">
-        <v>1.3720606769895567</v>
+        <v>0.49223821411253404</v>
       </c>
       <c r="AK8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL8" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>11</v>
@@ -1757,45 +1717,49 @@
     </row>
     <row r="9" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>183</v>
+        <v>620</v>
       </c>
       <c r="B9" s="6">
-        <v>15</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6" t="s">
-        <v>88</v>
+      <c r="J9" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="21" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="R9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es026_01_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="5">
         <v>0</v>
@@ -1840,16 +1804,16 @@
         <v>0</v>
       </c>
       <c r="AI9" s="6" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ9" s="7">
-        <v>1.4575910112359554</v>
+        <v>0.4435731398502184</v>
       </c>
       <c r="AK9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL9" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL9" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>11</v>
@@ -1871,43 +1835,45 @@
     </row>
     <row r="10" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>184</v>
+        <v>621</v>
       </c>
       <c r="B10" s="6">
-        <v>15</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="21">
+        <v>1</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="6" t="s">
-        <v>88</v>
+      <c r="J10" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="21" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="5" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="R10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es026_02_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="5">
         <v>0</v>
@@ -1952,16 +1918,16 @@
         <v>0</v>
       </c>
       <c r="AI10" s="6" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="AJ10" s="7">
-        <v>1.5296449438202244</v>
+        <v>0.46796696177456504</v>
       </c>
       <c r="AK10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL10" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL10" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>11</v>
@@ -1983,41 +1949,45 @@
     </row>
     <row r="11" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>185</v>
+        <v>622</v>
       </c>
       <c r="B11" s="6">
-        <v>14</v>
-      </c>
-      <c r="C11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>41</v>
+      <c r="C11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="21">
+        <v>1</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6" t="s">
-        <v>88</v>
+      <c r="J11" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="21">
+        <v>1</v>
+      </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="5" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="R11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es023_29_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S11" s="5"/>
       <c r="T11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="5">
         <v>0</v>
@@ -2062,16 +2032,16 @@
         <v>0</v>
       </c>
       <c r="AI11" s="6" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="AJ11" s="7">
-        <v>1.7387138318648576</v>
+        <v>0.48595800259460387</v>
       </c>
       <c r="AK11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL11" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL11" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>11</v>
@@ -2093,41 +2063,45 @@
     </row>
     <row r="12" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>186</v>
+        <v>623</v>
       </c>
       <c r="B12" s="6">
-        <v>14</v>
-      </c>
-      <c r="C12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>41</v>
+      <c r="C12" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="21">
+        <v>1</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
-        <v>88</v>
+      <c r="J12" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="21"/>
+      <c r="O12" s="21">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="5" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="R12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es023_30_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S12" s="5"/>
       <c r="T12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="5">
         <v>0</v>
@@ -2172,16 +2146,16 @@
         <v>0</v>
       </c>
       <c r="AI12" s="6" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="AJ12" s="7">
-        <v>1.7447145698523117</v>
+        <v>0.55592316133919994</v>
       </c>
       <c r="AK12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL12" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL12" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>11</v>
@@ -2203,41 +2177,45 @@
     </row>
     <row r="13" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>187</v>
+        <v>624</v>
       </c>
       <c r="B13" s="6">
-        <v>13</v>
-      </c>
-      <c r="C13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>41</v>
+      <c r="C13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="21">
+        <v>1</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
-        <v>88</v>
+      <c r="J13" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="21"/>
+      <c r="O13" s="21">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="5" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="R13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es014_20_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S13" s="5"/>
       <c r="T13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="5">
         <v>0</v>
@@ -2282,16 +2260,16 @@
         <v>0</v>
       </c>
       <c r="AI13" s="6" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="AJ13" s="7">
-        <v>1.6912604588394056</v>
+        <v>0.64188035636827412</v>
       </c>
       <c r="AK13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL13" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL13" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM13" s="5" t="s">
         <v>11</v>
@@ -2313,41 +2291,45 @@
     </row>
     <row r="14" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>188</v>
+        <v>625</v>
       </c>
       <c r="B14" s="6">
-        <v>14</v>
-      </c>
-      <c r="C14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>41</v>
+      <c r="C14" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="21">
+        <v>1</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>88</v>
+      <c r="J14" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="21"/>
+      <c r="O14" s="21">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="5" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="R14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es023_31_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="5">
         <v>0</v>
@@ -2392,16 +2374,16 @@
         <v>0</v>
       </c>
       <c r="AI14" s="6" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AJ14" s="7">
-        <v>1.4386769324921469</v>
+        <v>0.4799609889879245</v>
       </c>
       <c r="AK14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL14" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL14" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM14" s="5" t="s">
         <v>11</v>
@@ -2423,41 +2405,45 @@
     </row>
     <row r="15" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>189</v>
+        <v>626</v>
       </c>
       <c r="B15" s="6">
-        <v>14</v>
-      </c>
-      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>41</v>
+      <c r="C15" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="21">
+        <v>1</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6" t="s">
-        <v>88</v>
+      <c r="J15" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="21"/>
+      <c r="O15" s="21">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="5" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="R15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es023_32_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S15" s="5"/>
       <c r="T15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="5">
         <v>0</v>
@@ -2502,16 +2488,16 @@
         <v>0</v>
       </c>
       <c r="AI15" s="6" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="AJ15" s="7">
-        <v>1.6967086659526778</v>
+        <v>0.48995601166572411</v>
       </c>
       <c r="AK15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL15" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL15" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM15" s="5" t="s">
         <v>11</v>
@@ -2533,41 +2519,47 @@
     </row>
     <row r="16" spans="1:51" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>190</v>
+        <v>627</v>
       </c>
       <c r="B16" s="6">
-        <v>13</v>
-      </c>
-      <c r="C16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
-        <v>88</v>
+      <c r="J16" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="21"/>
+      <c r="O16" s="21">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="5" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="R16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es014_21_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="S16" s="5"/>
       <c r="T16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="5">
         <v>0</v>
@@ -2612,16 +2604,16 @@
         <v>0</v>
       </c>
       <c r="AI16" s="6" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="AJ16" s="7">
-        <v>3.113900134952766</v>
+        <v>0.52993610237692124</v>
       </c>
       <c r="AK16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL16" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AL16" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>11</v>
@@ -2641,348 +2633,8 @@
       <c r="AV16" s="5"/>
       <c r="AX16" s="25"/>
     </row>
-    <row r="17" spans="1:50" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>191</v>
-      </c>
-      <c r="B17" s="6">
-        <v>14</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="21">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_01_cc</v>
-      </c>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5">
-        <v>1</v>
-      </c>
-      <c r="U17" s="5">
-        <v>0</v>
-      </c>
-      <c r="V17" s="19">
-        <v>0</v>
-      </c>
-      <c r="W17" s="5">
-        <v>0</v>
-      </c>
-      <c r="X17" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ17" s="7">
-        <v>1.7269852934120529</v>
-      </c>
-      <c r="AK17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN17" s="9">
-        <v>2.8774999999999999</v>
-      </c>
-      <c r="AO17" s="8"/>
-      <c r="AP17" s="5"/>
-      <c r="AQ17" s="11">
-        <v>0.97727376388812615</v>
-      </c>
-      <c r="AR17" s="11"/>
-      <c r="AS17" s="11"/>
-      <c r="AT17" s="11"/>
-      <c r="AU17" s="11"/>
-      <c r="AV17" s="5"/>
-      <c r="AX17" s="25"/>
-    </row>
-    <row r="18" spans="1:50" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>192</v>
-      </c>
-      <c r="B18" s="6">
-        <v>14</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_02_cc</v>
-      </c>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5">
-        <v>1</v>
-      </c>
-      <c r="U18" s="5">
-        <v>0</v>
-      </c>
-      <c r="V18" s="19">
-        <v>0</v>
-      </c>
-      <c r="W18" s="5">
-        <v>0</v>
-      </c>
-      <c r="X18" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ18" s="7">
-        <v>1.7569937259648261</v>
-      </c>
-      <c r="AK18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN18" s="9">
-        <v>2.9275000000000011</v>
-      </c>
-      <c r="AO18" s="8"/>
-      <c r="AP18" s="5"/>
-      <c r="AQ18" s="11">
-        <v>0.99425506299999666</v>
-      </c>
-      <c r="AR18" s="11"/>
-      <c r="AS18" s="11"/>
-      <c r="AT18" s="11"/>
-      <c r="AU18" s="11"/>
-      <c r="AV18" s="5"/>
-      <c r="AX18" s="25"/>
-    </row>
-    <row r="19" spans="1:50" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>193</v>
-      </c>
-      <c r="B19" s="6">
-        <v>14</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_03_cc</v>
-      </c>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5">
-        <v>1</v>
-      </c>
-      <c r="U19" s="5">
-        <v>0</v>
-      </c>
-      <c r="V19" s="19">
-        <v>0</v>
-      </c>
-      <c r="W19" s="5">
-        <v>0</v>
-      </c>
-      <c r="X19" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ19" s="7">
-        <v>1.7149819203909447</v>
-      </c>
-      <c r="AK19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN19" s="9">
-        <v>2.8575000000000008</v>
-      </c>
-      <c r="AO19" s="8"/>
-      <c r="AP19" s="5"/>
-      <c r="AQ19" s="11">
-        <v>0.97048124424337856</v>
-      </c>
-      <c r="AR19" s="11"/>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="5"/>
-      <c r="AX19" s="25"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AY19"/>
+  <autoFilter ref="A1:AY16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2993,9 +2645,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C803"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3012,7 +2664,7 @@
         <v>Sr.No</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -3021,178 +2673,202 @@
         <v>Units</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>614</v>
+      </c>
       <c r="B3" s="25" t="str">
         <f>db_table!Q3</f>
-        <v>20131021_es024_01_cc</v>
+        <v>20160805_test001_45_cc</v>
       </c>
       <c r="C3" s="25" t="str">
-        <f t="shared" ref="C3:C19" si="0">CONCATENATE(B3,"_01.res")</f>
-        <v>20131021_es024_01_cc_01.res</v>
+        <f t="shared" ref="C3:C16" si="0">CONCATENATE(B3,"_01.res")</f>
+        <v>20160805_test001_45_cc_01.res</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>615</v>
+      </c>
       <c r="B4" s="25" t="str">
         <f>db_table!Q4</f>
-        <v>20131021_es024_02_cc</v>
+        <v>20160805_test001_46_cc</v>
       </c>
       <c r="C4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es024_02_cc_01.res</v>
+        <v>20160805_test001_46_cc_01.res</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>616</v>
+      </c>
       <c r="B5" s="25" t="str">
         <f>db_table!Q5</f>
-        <v>20131021_es024_03_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es024_03_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>617</v>
+      </c>
       <c r="B6" s="25" t="str">
         <f>db_table!Q6</f>
-        <v>20131021_es025_01_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C6" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_01_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>618</v>
+      </c>
       <c r="B7" s="25" t="str">
         <f>db_table!Q7</f>
-        <v>20131021_es025_02_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C7" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_02_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>619</v>
+      </c>
       <c r="B8" s="25" t="str">
         <f>db_table!Q8</f>
-        <v>20131021_es025_03_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C8" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es025_03_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>620</v>
+      </c>
       <c r="B9" s="25" t="str">
         <f>db_table!Q9</f>
-        <v>20131021_es026_01_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es026_01_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>621</v>
+      </c>
       <c r="B10" s="25" t="str">
         <f>db_table!Q10</f>
-        <v>20131021_es026_02_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131021_es026_02_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>622</v>
+      </c>
       <c r="B11" s="25" t="str">
         <f>db_table!Q11</f>
-        <v>20131025_es023_29_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es023_29_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>623</v>
+      </c>
       <c r="B12" s="25" t="str">
         <f>db_table!Q12</f>
-        <v>20131025_es023_30_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es023_30_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>624</v>
+      </c>
       <c r="B13" s="25" t="str">
         <f>db_table!Q13</f>
-        <v>20131025_es014_20_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131025_es014_20_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>625</v>
+      </c>
       <c r="B14" s="25" t="str">
         <f>db_table!Q14</f>
-        <v>20131029_es023_31_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C14" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es023_31_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>626</v>
+      </c>
       <c r="B15" s="25" t="str">
         <f>db_table!Q15</f>
-        <v>20131029_es023_32_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es023_32_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>627</v>
+      </c>
       <c r="B16" s="25" t="str">
         <f>db_table!Q16</f>
-        <v>20131029_es014_21_cc</v>
+        <v>20160805_test001_47_cc</v>
       </c>
       <c r="C16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>20131029_es014_21_cc_01.res</v>
+        <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="str">
-        <f>db_table!Q17</f>
-        <v>20131029_es027_01_cc</v>
-      </c>
-      <c r="C17" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_01_cc_01.res</v>
-      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="str">
-        <f>db_table!Q18</f>
-        <v>20131029_es027_02_cc</v>
-      </c>
-      <c r="C18" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_02_cc_01.res</v>
-      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="str">
-        <f>db_table!Q19</f>
-        <v>20131029_es027_03_cc</v>
-      </c>
-      <c r="C19" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>20131029_es027_03_cc_01.res</v>
-      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>

</xml_diff>

<commit_message>
add optional interpolation for ocv and voltage cycles
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jepe/scripting/cellpy/testdata/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581DD207-095C-5E43-BCD7-49076D3A03F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E181731A-B5B1-6844-B064-6A5B1177B543}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="7120" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -23,11 +23,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$AZ$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="85">
   <si>
     <t>(mg)</t>
   </si>
@@ -279,6 +286,9 @@
   </si>
   <si>
     <t>list</t>
+  </si>
+  <si>
+    <t>anode</t>
   </si>
 </sst>
 </file>
@@ -769,10 +779,10 @@
   <dimension ref="A1:BB16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AN3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR1" sqref="AR1"/>
+      <selection pane="bottomRight" activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1212,7 +1222,9 @@
       <c r="AJ3" s="7">
         <v>0.51026231569116942</v>
       </c>
-      <c r="AK3" s="7"/>
+      <c r="AK3" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1343,9 @@
       <c r="AJ4" s="7">
         <v>0.45438760079739932</v>
       </c>
-      <c r="AK4" s="7"/>
+      <c r="AK4" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1445,7 +1459,9 @@
       <c r="AJ5" s="7">
         <v>0.495843034428261</v>
       </c>
-      <c r="AK5" s="7"/>
+      <c r="AK5" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1562,7 +1578,9 @@
       <c r="AJ6" s="7">
         <v>0.45438760079739932</v>
       </c>
-      <c r="AK6" s="7"/>
+      <c r="AK6" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1677,7 +1695,9 @@
       <c r="AJ7" s="7">
         <v>0.44717796016594541</v>
       </c>
-      <c r="AK7" s="7"/>
+      <c r="AK7" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL7" s="5" t="s">
         <v>2</v>
       </c>
@@ -1792,7 +1812,9 @@
       <c r="AJ8" s="7">
         <v>0.49223821411253404</v>
       </c>
-      <c r="AK8" s="7"/>
+      <c r="AK8" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL8" s="5" t="s">
         <v>2</v>
       </c>
@@ -1911,7 +1933,9 @@
       <c r="AJ9" s="7">
         <v>0.4435731398502184</v>
       </c>
-      <c r="AK9" s="7"/>
+      <c r="AK9" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL9" s="5" t="s">
         <v>2</v>
       </c>
@@ -2026,7 +2050,9 @@
       <c r="AJ10" s="7">
         <v>0.46796696177456504</v>
       </c>
-      <c r="AK10" s="7"/>
+      <c r="AK10" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL10" s="5" t="s">
         <v>2</v>
       </c>
@@ -2141,7 +2167,9 @@
       <c r="AJ11" s="7">
         <v>0.48595800259460387</v>
       </c>
-      <c r="AK11" s="7"/>
+      <c r="AK11" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL11" s="5" t="s">
         <v>2</v>
       </c>
@@ -2256,7 +2284,9 @@
       <c r="AJ12" s="7">
         <v>0.55592316133919994</v>
       </c>
-      <c r="AK12" s="7"/>
+      <c r="AK12" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL12" s="5" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2401,9 @@
       <c r="AJ13" s="7">
         <v>0.64188035636827412</v>
       </c>
-      <c r="AK13" s="7"/>
+      <c r="AK13" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL13" s="5" t="s">
         <v>2</v>
       </c>
@@ -2486,7 +2518,9 @@
       <c r="AJ14" s="7">
         <v>0.4799609889879245</v>
       </c>
-      <c r="AK14" s="7"/>
+      <c r="AK14" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL14" s="5" t="s">
         <v>2</v>
       </c>
@@ -2601,7 +2635,9 @@
       <c r="AJ15" s="7">
         <v>0.48995601166572411</v>
       </c>
-      <c r="AK15" s="7"/>
+      <c r="AK15" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL15" s="5" t="s">
         <v>2</v>
       </c>
@@ -2718,7 +2754,9 @@
       <c r="AJ16" s="7">
         <v>0.52993610237692124</v>
       </c>
-      <c r="AK16" s="7"/>
+      <c r="AK16" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="AL16" s="5" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
xlrd has explicitly removed support for anything other than xls files. depend on openpyxl insted.
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jepe/scripting/cellpy/testdata/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripts\cellpy\testdata\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33BF0AA-F617-F34B-AC75-FD68A7ABC37B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6566EC46-6603-47D0-A2EE-3957778144D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2655" windowWidth="29040" windowHeight="15840" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -419,7 +421,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -749,49 +751,49 @@
       <selection pane="bottomRight" activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="14" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" style="22" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="22" customWidth="1"/>
     <col min="7" max="9" width="10" style="2" customWidth="1"/>
-    <col min="10" max="12" width="7.83203125" style="2" customWidth="1"/>
+    <col min="10" max="12" width="7.81640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="9" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" style="22" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="39.33203125" customWidth="1"/>
-    <col min="18" max="18" width="27.5" customWidth="1"/>
-    <col min="19" max="19" width="59.33203125" customWidth="1"/>
-    <col min="20" max="20" width="10.5" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="22" max="22" width="7.1640625" style="20" customWidth="1"/>
-    <col min="23" max="23" width="7.1640625" customWidth="1"/>
-    <col min="24" max="24" width="7.1640625" style="16" customWidth="1"/>
-    <col min="25" max="25" width="7.1640625" customWidth="1"/>
-    <col min="26" max="26" width="7.1640625" style="18" customWidth="1"/>
-    <col min="27" max="27" width="7.1640625" customWidth="1"/>
-    <col min="28" max="28" width="7.1640625" style="24" customWidth="1"/>
-    <col min="29" max="34" width="7.1640625" customWidth="1"/>
-    <col min="35" max="35" width="16.83203125" style="2" customWidth="1"/>
-    <col min="36" max="37" width="14.5" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.36328125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.1796875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="21.6328125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="39.36328125" customWidth="1"/>
+    <col min="18" max="18" width="27.453125" customWidth="1"/>
+    <col min="19" max="19" width="59.36328125" customWidth="1"/>
+    <col min="20" max="20" width="10.453125" customWidth="1"/>
+    <col min="21" max="21" width="10.6328125" customWidth="1"/>
+    <col min="22" max="22" width="7.1796875" style="20" customWidth="1"/>
+    <col min="23" max="23" width="7.1796875" customWidth="1"/>
+    <col min="24" max="24" width="7.1796875" style="16" customWidth="1"/>
+    <col min="25" max="25" width="7.1796875" customWidth="1"/>
+    <col min="26" max="26" width="7.1796875" style="18" customWidth="1"/>
+    <col min="27" max="27" width="7.1796875" customWidth="1"/>
+    <col min="28" max="28" width="7.1796875" style="24" customWidth="1"/>
+    <col min="29" max="34" width="7.1796875" customWidth="1"/>
+    <col min="35" max="35" width="16.81640625" style="2" customWidth="1"/>
+    <col min="36" max="37" width="14.453125" style="4" customWidth="1"/>
     <col min="38" max="38" width="10" customWidth="1"/>
-    <col min="39" max="39" width="12.33203125" customWidth="1"/>
-    <col min="40" max="40" width="13.83203125" customWidth="1"/>
-    <col min="41" max="41" width="17.5" style="10" customWidth="1"/>
-    <col min="42" max="42" width="9.1640625" style="3" customWidth="1"/>
-    <col min="43" max="43" width="5.83203125" customWidth="1"/>
+    <col min="39" max="39" width="12.36328125" customWidth="1"/>
+    <col min="40" max="40" width="13.81640625" customWidth="1"/>
+    <col min="41" max="41" width="17.453125" style="10" customWidth="1"/>
+    <col min="42" max="42" width="9.1796875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="5.81640625" customWidth="1"/>
     <col min="44" max="44" width="29" style="12" customWidth="1"/>
-    <col min="45" max="47" width="8.1640625" style="12" customWidth="1"/>
-    <col min="48" max="48" width="29.1640625" style="12" customWidth="1"/>
+    <col min="45" max="47" width="8.1796875" style="12" customWidth="1"/>
+    <col min="48" max="48" width="29.1796875" style="12" customWidth="1"/>
     <col min="49" max="49" width="110" customWidth="1"/>
-    <col min="50" max="50" width="8.5" customWidth="1"/>
+    <col min="50" max="50" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
@@ -942,7 +944,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>614</v>
       </c>
@@ -1215,7 +1217,7 @@
       </c>
       <c r="AY3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>615</v>
       </c>
@@ -1334,7 +1336,7 @@
       <c r="AW4" s="5"/>
       <c r="AY4" s="25"/>
     </row>
-    <row r="5" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>616</v>
       </c>
@@ -1450,7 +1452,7 @@
       <c r="AW5" s="5"/>
       <c r="AY5" s="25"/>
     </row>
-    <row r="6" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>617</v>
       </c>
@@ -1569,7 +1571,7 @@
       <c r="AW6" s="5"/>
       <c r="AY6" s="25"/>
     </row>
-    <row r="7" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>618</v>
       </c>
@@ -1686,7 +1688,7 @@
       <c r="AW7" s="5"/>
       <c r="AY7" s="25"/>
     </row>
-    <row r="8" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>619</v>
       </c>
@@ -1803,7 +1805,7 @@
       <c r="AW8" s="5"/>
       <c r="AY8" s="25"/>
     </row>
-    <row r="9" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>620</v>
       </c>
@@ -1924,7 +1926,7 @@
       <c r="AW9" s="5"/>
       <c r="AY9" s="25"/>
     </row>
-    <row r="10" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>621</v>
       </c>
@@ -2041,7 +2043,7 @@
       <c r="AW10" s="5"/>
       <c r="AY10" s="25"/>
     </row>
-    <row r="11" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>622</v>
       </c>
@@ -2158,7 +2160,7 @@
       <c r="AW11" s="5"/>
       <c r="AY11" s="25"/>
     </row>
-    <row r="12" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>623</v>
       </c>
@@ -2275,7 +2277,7 @@
       <c r="AW12" s="5"/>
       <c r="AY12" s="25"/>
     </row>
-    <row r="13" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>624</v>
       </c>
@@ -2392,7 +2394,7 @@
       <c r="AW13" s="5"/>
       <c r="AY13" s="25"/>
     </row>
-    <row r="14" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>625</v>
       </c>
@@ -2509,7 +2511,7 @@
       <c r="AW14" s="5"/>
       <c r="AY14" s="25"/>
     </row>
-    <row r="15" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>626</v>
       </c>
@@ -2626,7 +2628,7 @@
       <c r="AW15" s="5"/>
       <c r="AY15" s="25"/>
     </row>
-    <row r="16" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>627</v>
       </c>
@@ -2762,15 +2764,15 @@
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="9" width="36.5" customWidth="1"/>
-    <col min="10" max="19" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="9" width="36.453125" customWidth="1"/>
+    <col min="10" max="19" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>85</v>
       </c>
@@ -2778,7 +2780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>86</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>614</v>
       </c>
@@ -2799,7 +2801,7 @@
         <v>20160805_test001_45_cc_01.res</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>615</v>
       </c>
@@ -2812,7 +2814,7 @@
         <v>20160805_test001_46_cc_01.res</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>616</v>
       </c>
@@ -2825,7 +2827,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>617</v>
       </c>
@@ -2838,7 +2840,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>618</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>619</v>
       </c>
@@ -2864,7 +2866,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>620</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>621</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>622</v>
       </c>
@@ -2903,7 +2905,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>623</v>
       </c>
@@ -2916,7 +2918,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>624</v>
       </c>
@@ -2929,7 +2931,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>625</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>626</v>
       </c>
@@ -2955,7 +2957,7 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>627</v>
       </c>
@@ -2968,825 +2970,826 @@
         <v>20160805_test001_47_cc_01.res</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
     </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B20" s="25"/>
     </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B21" s="25"/>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B22" s="25"/>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B24" s="25"/>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B25" s="25"/>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B26" s="25"/>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B27" s="25"/>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B28" s="25"/>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B29" s="25"/>
     </row>
-    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="609" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="610" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="611" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="612" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="613" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="614" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="615" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:3" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:3" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="41" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="42" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="43" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="46" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="68" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="69" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="74" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="77" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="609" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="610" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="611" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="612" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="613" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="614" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="615" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A615" s="5"/>
     </row>
-    <row r="616" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="617" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="618" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="619" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="620" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="621" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="622" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="623" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="624" spans="1:1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="616" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="617" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="618" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="619" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="620" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="621" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="622" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="623" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="624" spans="1:1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add "instrument" to db testfile (xlsx)
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripts\cellpy\testdata\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripting\cellpy\testdata\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930D32CC-1CB2-4CA2-B18D-61AEBB8A200F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2860B3B-3D9D-49DD-B0E0-DD664E209BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="db_filenames" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$AZ$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$BA$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="89">
   <si>
     <t>(mg)</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>Units</t>
+  </si>
+  <si>
+    <t>instrument</t>
+  </si>
+  <si>
+    <t>arbin_res</t>
   </si>
 </sst>
 </file>
@@ -742,13 +748,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:BB16"/>
+  <dimension ref="A1:BC16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,19 +787,20 @@
     <col min="35" max="35" width="16.85546875" style="2" customWidth="1"/>
     <col min="36" max="37" width="14.42578125" style="4" customWidth="1"/>
     <col min="38" max="38" width="10" customWidth="1"/>
-    <col min="39" max="39" width="12.42578125" customWidth="1"/>
-    <col min="40" max="40" width="13.85546875" customWidth="1"/>
-    <col min="41" max="41" width="17.42578125" style="10" customWidth="1"/>
-    <col min="42" max="42" width="9.140625" style="3" customWidth="1"/>
-    <col min="43" max="43" width="5.85546875" customWidth="1"/>
-    <col min="44" max="44" width="29" style="12" customWidth="1"/>
-    <col min="45" max="47" width="8.140625" style="12" customWidth="1"/>
-    <col min="48" max="48" width="29.140625" style="12" customWidth="1"/>
-    <col min="49" max="49" width="110" customWidth="1"/>
-    <col min="50" max="50" width="8.42578125" customWidth="1"/>
+    <col min="39" max="39" width="10" style="25" customWidth="1"/>
+    <col min="40" max="40" width="12.42578125" customWidth="1"/>
+    <col min="41" max="41" width="13.85546875" customWidth="1"/>
+    <col min="42" max="42" width="17.42578125" style="10" customWidth="1"/>
+    <col min="43" max="43" width="9.140625" style="3" customWidth="1"/>
+    <col min="44" max="44" width="5.85546875" customWidth="1"/>
+    <col min="45" max="45" width="29" style="12" customWidth="1"/>
+    <col min="46" max="48" width="8.140625" style="12" customWidth="1"/>
+    <col min="49" max="49" width="29.140625" style="12" customWidth="1"/>
+    <col min="50" max="50" width="110" customWidth="1"/>
+    <col min="51" max="51" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
@@ -909,42 +916,45 @@
         <v>67</v>
       </c>
       <c r="AM1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AP1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="11" t="s">
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="AS1" s="11"/>
       <c r="AT1" s="11"/>
       <c r="AU1" s="11"/>
-      <c r="AV1" s="11" t="s">
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>72</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>73</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>77</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -1065,38 +1075,41 @@
       <c r="AN2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AO2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="11" t="s">
+      <c r="AO2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AS2" s="11"/>
       <c r="AT2" s="11"/>
       <c r="AU2" s="11"/>
-      <c r="AV2" s="11" t="s">
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AX2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>4</v>
       </c>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" t="s">
+      <c r="AZ2" s="25"/>
+      <c r="BA2" t="s">
         <v>82</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>83</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>614</v>
       </c>
@@ -1195,29 +1208,32 @@
         <v>2</v>
       </c>
       <c r="AM3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN3" s="5" t="s">
+      <c r="AO3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO3" s="9">
+      <c r="AP3" s="9">
         <v>2.8174999999999999</v>
       </c>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="11">
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="11">
         <v>0.95636867792127611</v>
       </c>
-      <c r="AS3" s="11"/>
       <c r="AT3" s="11"/>
       <c r="AU3" s="11"/>
       <c r="AV3" s="11"/>
-      <c r="AW3" s="5" t="s">
+      <c r="AW3" s="11"/>
+      <c r="AX3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AY3" s="25"/>
-    </row>
-    <row r="4" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="25"/>
+    </row>
+    <row r="4" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>615</v>
       </c>
@@ -1316,27 +1332,30 @@
         <v>2</v>
       </c>
       <c r="AM4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN4" s="5" t="s">
+      <c r="AO4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO4" s="9">
+      <c r="AP4" s="9">
         <v>2.5374999999999996</v>
       </c>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="11">
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="11">
         <v>0.86132582794152224</v>
       </c>
-      <c r="AS4" s="11"/>
       <c r="AT4" s="11"/>
       <c r="AU4" s="11"/>
       <c r="AV4" s="11"/>
-      <c r="AW4" s="5"/>
-      <c r="AY4" s="25"/>
-    </row>
-    <row r="5" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW4" s="11"/>
+      <c r="AX4" s="5"/>
+      <c r="AZ4" s="25"/>
+    </row>
+    <row r="5" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>616</v>
       </c>
@@ -1432,27 +1451,30 @@
         <v>2</v>
       </c>
       <c r="AM5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AO5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO5" s="9">
+      <c r="AP5" s="9">
         <v>2.6975000000000002</v>
       </c>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="11">
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="11">
         <v>0.91563602792995336</v>
       </c>
-      <c r="AS5" s="11"/>
       <c r="AT5" s="11"/>
       <c r="AU5" s="11"/>
       <c r="AV5" s="11"/>
-      <c r="AW5" s="5"/>
-      <c r="AY5" s="25"/>
-    </row>
-    <row r="6" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW5" s="11"/>
+      <c r="AX5" s="5"/>
+      <c r="AZ5" s="25"/>
+    </row>
+    <row r="6" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>617</v>
       </c>
@@ -1551,27 +1573,30 @@
         <v>2</v>
       </c>
       <c r="AM6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN6" s="5" t="s">
+      <c r="AO6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO6" s="9">
+      <c r="AP6" s="9">
         <v>2.8974999999999991</v>
       </c>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="11">
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="11">
         <v>0.98347485400488432</v>
       </c>
-      <c r="AS6" s="11"/>
       <c r="AT6" s="11"/>
       <c r="AU6" s="11"/>
       <c r="AV6" s="11"/>
-      <c r="AW6" s="5"/>
-      <c r="AY6" s="25"/>
-    </row>
-    <row r="7" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="5"/>
+      <c r="AZ6" s="25"/>
+    </row>
+    <row r="7" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>618</v>
       </c>
@@ -1668,27 +1693,30 @@
         <v>2</v>
       </c>
       <c r="AM7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN7" s="5" t="s">
+      <c r="AO7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO7" s="9">
+      <c r="AP7" s="9">
         <v>2.7875000000000001</v>
       </c>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="11">
+      <c r="AQ7" s="8"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="11">
         <v>0.94613844884852993</v>
       </c>
-      <c r="AS7" s="11"/>
       <c r="AT7" s="11"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
-      <c r="AW7" s="5"/>
-      <c r="AY7" s="25"/>
-    </row>
-    <row r="8" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW7" s="11"/>
+      <c r="AX7" s="5"/>
+      <c r="AZ7" s="25"/>
+    </row>
+    <row r="8" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>619</v>
       </c>
@@ -1785,27 +1813,30 @@
         <v>2</v>
       </c>
       <c r="AM8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO8" s="9">
+      <c r="AP8" s="9">
         <v>2.2874999999999996</v>
       </c>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="11">
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="11">
         <v>0.77642751631964557</v>
       </c>
-      <c r="AS8" s="11"/>
       <c r="AT8" s="11"/>
       <c r="AU8" s="11"/>
       <c r="AV8" s="11"/>
-      <c r="AW8" s="5"/>
-      <c r="AY8" s="25"/>
-    </row>
-    <row r="9" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW8" s="11"/>
+      <c r="AX8" s="5"/>
+      <c r="AZ8" s="25"/>
+    </row>
+    <row r="9" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>620</v>
       </c>
@@ -1906,27 +1937,30 @@
         <v>2</v>
       </c>
       <c r="AM9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN9" s="5" t="s">
+      <c r="AO9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO9" s="9">
+      <c r="AP9" s="9">
         <v>2.4275000000000007</v>
       </c>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="11">
+      <c r="AQ9" s="8"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="11">
         <v>0.82482778469161488</v>
       </c>
-      <c r="AS9" s="11"/>
       <c r="AT9" s="11"/>
       <c r="AU9" s="11"/>
       <c r="AV9" s="11"/>
-      <c r="AW9" s="5"/>
-      <c r="AY9" s="25"/>
-    </row>
-    <row r="10" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW9" s="11"/>
+      <c r="AX9" s="5"/>
+      <c r="AZ9" s="25"/>
+    </row>
+    <row r="10" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>621</v>
       </c>
@@ -2023,27 +2057,30 @@
         <v>2</v>
       </c>
       <c r="AM10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN10" s="5" t="s">
+      <c r="AO10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO10" s="9">
+      <c r="AP10" s="9">
         <v>2.5474999999999994</v>
       </c>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="11">
+      <c r="AQ10" s="8"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="11">
         <v>0.86560196972271386</v>
       </c>
-      <c r="AS10" s="11"/>
       <c r="AT10" s="11"/>
       <c r="AU10" s="11"/>
       <c r="AV10" s="11"/>
-      <c r="AW10" s="5"/>
-      <c r="AY10" s="25"/>
-    </row>
-    <row r="11" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW10" s="11"/>
+      <c r="AX10" s="5"/>
+      <c r="AZ10" s="25"/>
+    </row>
+    <row r="11" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>622</v>
       </c>
@@ -2140,27 +2177,30 @@
         <v>2</v>
       </c>
       <c r="AM11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN11" s="5" t="s">
+      <c r="AO11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO11" s="9">
+      <c r="AP11" s="9">
         <v>2.8974999999999991</v>
       </c>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="11">
+      <c r="AQ11" s="8"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="11">
         <v>0.98391075898148517</v>
       </c>
-      <c r="AS11" s="11"/>
       <c r="AT11" s="11"/>
       <c r="AU11" s="11"/>
       <c r="AV11" s="11"/>
-      <c r="AW11" s="5"/>
-      <c r="AY11" s="25"/>
-    </row>
-    <row r="12" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="5"/>
+      <c r="AZ11" s="25"/>
+    </row>
+    <row r="12" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>623</v>
       </c>
@@ -2257,27 +2297,30 @@
         <v>2</v>
       </c>
       <c r="AM12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN12" s="5" t="s">
+      <c r="AO12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO12" s="9">
+      <c r="AP12" s="9">
         <v>2.9074999999999984</v>
       </c>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="11">
+      <c r="AQ12" s="8"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="11">
         <v>0.98730648204958338</v>
       </c>
-      <c r="AS12" s="11"/>
       <c r="AT12" s="11"/>
       <c r="AU12" s="11"/>
       <c r="AV12" s="11"/>
-      <c r="AW12" s="5"/>
-      <c r="AY12" s="25"/>
-    </row>
-    <row r="13" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW12" s="11"/>
+      <c r="AX12" s="5"/>
+      <c r="AZ12" s="25"/>
+    </row>
+    <row r="13" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>624</v>
       </c>
@@ -2374,27 +2417,30 @@
         <v>2</v>
       </c>
       <c r="AM13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN13" s="5" t="s">
+      <c r="AO13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO13" s="9">
+      <c r="AP13" s="9">
         <v>2.817499999999999</v>
       </c>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="11">
+      <c r="AQ13" s="8"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="11">
         <v>0.95705764295167428</v>
       </c>
-      <c r="AS13" s="11"/>
       <c r="AT13" s="11"/>
       <c r="AU13" s="11"/>
       <c r="AV13" s="11"/>
-      <c r="AW13" s="5"/>
-      <c r="AY13" s="25"/>
-    </row>
-    <row r="14" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW13" s="11"/>
+      <c r="AX13" s="5"/>
+      <c r="AZ13" s="25"/>
+    </row>
+    <row r="14" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>625</v>
       </c>
@@ -2491,27 +2537,30 @@
         <v>2</v>
       </c>
       <c r="AM14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN14" s="5" t="s">
+      <c r="AO14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO14" s="9">
+      <c r="AP14" s="9">
         <v>2.3974999999999986</v>
       </c>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="5"/>
-      <c r="AR14" s="11">
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="11">
         <v>0.81412460557656952</v>
       </c>
-      <c r="AS14" s="11"/>
       <c r="AT14" s="11"/>
       <c r="AU14" s="11"/>
       <c r="AV14" s="11"/>
-      <c r="AW14" s="5"/>
-      <c r="AY14" s="25"/>
-    </row>
-    <row r="15" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW14" s="11"/>
+      <c r="AX14" s="5"/>
+      <c r="AZ14" s="25"/>
+    </row>
+    <row r="15" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>626</v>
       </c>
@@ -2608,27 +2657,30 @@
         <v>2</v>
       </c>
       <c r="AM15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN15" s="5" t="s">
+      <c r="AO15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO15" s="9">
+      <c r="AP15" s="9">
         <v>2.8274999999999983</v>
       </c>
-      <c r="AP15" s="8"/>
-      <c r="AQ15" s="5"/>
-      <c r="AR15" s="11">
+      <c r="AQ15" s="8"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="11">
         <v>0.96014069750479669</v>
       </c>
-      <c r="AS15" s="11"/>
       <c r="AT15" s="11"/>
       <c r="AU15" s="11"/>
       <c r="AV15" s="11"/>
-      <c r="AW15" s="5"/>
-      <c r="AY15" s="25"/>
-    </row>
-    <row r="16" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW15" s="11"/>
+      <c r="AX15" s="5"/>
+      <c r="AZ15" s="25"/>
+    </row>
+    <row r="16" spans="1:55" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>627</v>
       </c>
@@ -2727,28 +2779,31 @@
         <v>2</v>
       </c>
       <c r="AM16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN16" s="5" t="s">
+      <c r="AO16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AO16" s="9">
+      <c r="AP16" s="9">
         <v>5.1874999999999991</v>
       </c>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="5"/>
-      <c r="AR16" s="11">
+      <c r="AQ16" s="8"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="11">
         <v>1.7621070178568985</v>
       </c>
-      <c r="AS16" s="11"/>
       <c r="AT16" s="11"/>
       <c r="AU16" s="11"/>
       <c r="AV16" s="11"/>
-      <c r="AW16" s="5"/>
-      <c r="AY16" s="25"/>
+      <c r="AW16" s="11"/>
+      <c r="AX16" s="5"/>
+      <c r="AZ16" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AZ16" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:BA16" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
start to add more tests journal loading
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripting\cellpy\testdata\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC11AD-A7A7-4E11-859E-002B9DFD1629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98A0C97-6E10-4370-924B-E9B754A10839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5796" yWindow="1728" windowWidth="12696" windowHeight="10104" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17640" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -314,7 +314,7 @@
     <t>recalc=True</t>
   </si>
   <si>
-    <t>recalc=False</t>
+    <t>recalc=False;data_points=(1, 10000)</t>
   </si>
 </sst>
 </file>
@@ -771,51 +771,51 @@
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="14" customWidth="1"/>
     <col min="4" max="4" width="23" style="22" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="22" customWidth="1"/>
     <col min="8" max="10" width="10" style="2" customWidth="1"/>
-    <col min="11" max="13" width="7.88671875" style="2" customWidth="1"/>
+    <col min="11" max="13" width="7.85546875" style="2" customWidth="1"/>
     <col min="14" max="14" width="9" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" style="22" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="39.44140625" customWidth="1"/>
-    <col min="19" max="19" width="27.44140625" customWidth="1"/>
-    <col min="20" max="20" width="59.44140625" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" style="20" customWidth="1"/>
-    <col min="24" max="24" width="7.109375" customWidth="1"/>
-    <col min="25" max="25" width="7.109375" style="16" customWidth="1"/>
-    <col min="26" max="26" width="7.109375" customWidth="1"/>
-    <col min="27" max="27" width="7.109375" style="18" customWidth="1"/>
-    <col min="28" max="28" width="7.109375" customWidth="1"/>
-    <col min="29" max="29" width="7.109375" style="24" customWidth="1"/>
-    <col min="30" max="35" width="7.109375" customWidth="1"/>
-    <col min="36" max="36" width="16.88671875" style="2" customWidth="1"/>
-    <col min="37" max="38" width="14.44140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" style="22" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="39.42578125" customWidth="1"/>
+    <col min="19" max="19" width="27.42578125" customWidth="1"/>
+    <col min="20" max="20" width="59.42578125" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="20" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" customWidth="1"/>
+    <col min="25" max="25" width="7.140625" style="16" customWidth="1"/>
+    <col min="26" max="26" width="7.140625" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" style="18" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" customWidth="1"/>
+    <col min="29" max="29" width="7.140625" style="24" customWidth="1"/>
+    <col min="30" max="35" width="7.140625" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" style="2" customWidth="1"/>
+    <col min="37" max="38" width="14.42578125" style="4" customWidth="1"/>
     <col min="39" max="39" width="10" customWidth="1"/>
     <col min="40" max="40" width="10" style="25" customWidth="1"/>
-    <col min="41" max="41" width="12.44140625" customWidth="1"/>
-    <col min="42" max="42" width="13.88671875" customWidth="1"/>
-    <col min="43" max="43" width="17.44140625" style="10" customWidth="1"/>
-    <col min="44" max="44" width="9.109375" style="3" customWidth="1"/>
-    <col min="45" max="45" width="5.88671875" customWidth="1"/>
+    <col min="41" max="41" width="12.42578125" customWidth="1"/>
+    <col min="42" max="42" width="13.85546875" customWidth="1"/>
+    <col min="43" max="43" width="17.42578125" style="10" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="3" customWidth="1"/>
+    <col min="45" max="45" width="5.85546875" customWidth="1"/>
     <col min="46" max="46" width="29" style="12" customWidth="1"/>
-    <col min="47" max="49" width="8.109375" style="12" customWidth="1"/>
-    <col min="50" max="50" width="29.109375" style="12" customWidth="1"/>
+    <col min="47" max="49" width="8.140625" style="12" customWidth="1"/>
+    <col min="50" max="50" width="29.140625" style="12" customWidth="1"/>
     <col min="51" max="51" width="110" customWidth="1"/>
-    <col min="52" max="52" width="8.44140625" customWidth="1"/>
+    <col min="52" max="52" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>41</v>
       </c>
@@ -972,7 +972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>76</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>614</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="BA3" s="25"/>
     </row>
-    <row r="4" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>615</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="AY4" s="5"/>
       <c r="BA4" s="25"/>
     </row>
-    <row r="5" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>616</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="AY5" s="5"/>
       <c r="BA5" s="25"/>
     </row>
-    <row r="6" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>617</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="AY6" s="5"/>
       <c r="BA6" s="25"/>
     </row>
-    <row r="7" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>618</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="AY7" s="5"/>
       <c r="BA7" s="25"/>
     </row>
-    <row r="8" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>619</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="AY8" s="5"/>
       <c r="BA8" s="25"/>
     </row>
-    <row r="9" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>620</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="AY9" s="5"/>
       <c r="BA9" s="25"/>
     </row>
-    <row r="10" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>621</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="AY10" s="5"/>
       <c r="BA10" s="25"/>
     </row>
-    <row r="11" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>622</v>
       </c>
@@ -2240,7 +2240,7 @@
       <c r="AY11" s="5"/>
       <c r="BA11" s="25"/>
     </row>
-    <row r="12" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>623</v>
       </c>
@@ -2361,7 +2361,7 @@
       <c r="AY12" s="5"/>
       <c r="BA12" s="25"/>
     </row>
-    <row r="13" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>624</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="AY13" s="5"/>
       <c r="BA13" s="25"/>
     </row>
-    <row r="14" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>625</v>
       </c>
@@ -2603,7 +2603,7 @@
       <c r="AY14" s="5"/>
       <c r="BA14" s="25"/>
     </row>
-    <row r="15" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>626</v>
       </c>
@@ -2724,7 +2724,7 @@
       <c r="AY15" s="5"/>
       <c r="BA15" s="25"/>
     </row>
-    <row r="16" spans="1:56" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>627</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="AY16" s="5"/>
       <c r="BA16" s="25"/>
     </row>
-    <row r="17" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>628</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="BF17" s="1"/>
       <c r="BG17" s="1"/>
     </row>
-    <row r="18" spans="1:59" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:59" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>629</v>
       </c>
@@ -3092,7 +3092,7 @@
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
     </row>
-    <row r="19" spans="1:59" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:59" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>630</v>
       </c>

</xml_diff>

<commit_message>
not using pandas 2.2
</commit_message>
<xml_diff>
--- a/testdata/db/cellpy_db.xlsx
+++ b/testdata/db/cellpy_db.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripting\cellpy\testdata\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053BBF7E-44E3-4A3A-A54B-0F0B9F919DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B62B055-1D51-49E9-9786-3CD29836E576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17640" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$BB$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">db_table!$A$1:$BD$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="100">
   <si>
     <t>(mg)</t>
   </si>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>(cm^2)</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>experiment_type</t>
+  </si>
+  <si>
+    <t>cycling</t>
+  </si>
+  <si>
+    <t>nominal_capacity</t>
   </si>
 </sst>
 </file>
@@ -443,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -483,9 +495,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,26 +530,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,26 +565,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,59 +742,59 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:BD19"/>
+  <dimension ref="A1:BF19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT8" sqref="AT8"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="11" customWidth="1"/>
     <col min="4" max="4" width="23" style="19" customWidth="1"/>
     <col min="5" max="5" width="5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="19" customWidth="1"/>
     <col min="8" max="10" width="10" style="1" customWidth="1"/>
-    <col min="11" max="13" width="7.88671875" style="1" customWidth="1"/>
+    <col min="11" max="13" width="7.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" style="19" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="39.44140625" customWidth="1"/>
-    <col min="19" max="19" width="27.44140625" customWidth="1"/>
-    <col min="20" max="20" width="59.44140625" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" style="17" customWidth="1"/>
-    <col min="24" max="24" width="7.109375" customWidth="1"/>
-    <col min="25" max="25" width="7.109375" style="13" customWidth="1"/>
-    <col min="26" max="26" width="7.109375" customWidth="1"/>
-    <col min="27" max="27" width="7.109375" style="15" customWidth="1"/>
-    <col min="28" max="28" width="7.109375" customWidth="1"/>
-    <col min="29" max="29" width="7.109375" style="21" customWidth="1"/>
-    <col min="30" max="35" width="7.109375" customWidth="1"/>
-    <col min="36" max="36" width="16.88671875" style="1" customWidth="1"/>
-    <col min="37" max="38" width="14.44140625" style="2" customWidth="1"/>
-    <col min="39" max="40" width="10" customWidth="1"/>
-    <col min="41" max="41" width="12.44140625" customWidth="1"/>
-    <col min="42" max="42" width="13.88671875" customWidth="1"/>
-    <col min="43" max="43" width="17.44140625" style="7" customWidth="1"/>
-    <col min="44" max="44" width="9.109375" style="9" customWidth="1"/>
-    <col min="45" max="45" width="5.88671875" customWidth="1"/>
-    <col min="46" max="46" width="29" style="9" customWidth="1"/>
-    <col min="47" max="49" width="8.109375" style="9" customWidth="1"/>
-    <col min="50" max="50" width="29.109375" style="9" customWidth="1"/>
-    <col min="51" max="51" width="110" customWidth="1"/>
-    <col min="52" max="52" width="8.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="17.140625" style="19" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="39.42578125" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" customWidth="1"/>
+    <col min="21" max="21" width="59.42578125" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" style="17" customWidth="1"/>
+    <col min="25" max="25" width="7.140625" customWidth="1"/>
+    <col min="26" max="26" width="7.140625" style="13" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" style="15" customWidth="1"/>
+    <col min="29" max="29" width="7.140625" customWidth="1"/>
+    <col min="30" max="30" width="7.140625" style="21" customWidth="1"/>
+    <col min="31" max="36" width="7.140625" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" style="1" customWidth="1"/>
+    <col min="38" max="40" width="14.42578125" style="2" customWidth="1"/>
+    <col min="41" max="42" width="10" customWidth="1"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1"/>
+    <col min="44" max="44" width="13.85546875" customWidth="1"/>
+    <col min="45" max="45" width="17.42578125" style="7" customWidth="1"/>
+    <col min="46" max="46" width="9.140625" style="9" customWidth="1"/>
+    <col min="47" max="47" width="5.85546875" customWidth="1"/>
+    <col min="48" max="48" width="29" style="9" customWidth="1"/>
+    <col min="49" max="51" width="8.140625" style="9" customWidth="1"/>
+    <col min="52" max="52" width="29.140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="110" customWidth="1"/>
+    <col min="54" max="54" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -865,117 +843,123 @@
       <c r="P1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AD1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="8" t="s">
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
       <c r="AW1" s="8"/>
-      <c r="AX1" s="8" t="s">
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>70</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>71</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>75</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
@@ -1024,11 +1008,11 @@
       <c r="P2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>77</v>
@@ -1037,33 +1021,33 @@
         <v>77</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="W2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Y2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AC2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="AE2" s="3" t="s">
@@ -1081,17 +1065,17 @@
       <c r="AI2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AK2" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="AL2" s="5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>78</v>
@@ -1102,39 +1086,45 @@
       <c r="AP2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AQ2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="8" t="s">
+      <c r="AQ2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="8" t="s">
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
       <c r="AW2" s="8"/>
-      <c r="AX2" s="8" t="s">
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BB2" t="s">
         <v>4</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
         <v>80</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BE2" t="s">
         <v>81</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BF2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>614</v>
       </c>
@@ -1171,43 +1161,43 @@
       <c r="P3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="3" t="s">
+      <c r="Q3" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="3" t="str">
-        <f t="shared" ref="S3:S16" si="0">R3</f>
+      <c r="T3" s="3" t="str">
+        <f t="shared" ref="T3:T16" si="0">S3</f>
         <v>20160805_test001_45_cc</v>
       </c>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3">
-        <v>1</v>
-      </c>
+      <c r="U3" s="3"/>
       <c r="V3" s="3">
         <v>1</v>
       </c>
-      <c r="W3" s="16">
-        <v>0</v>
-      </c>
-      <c r="X3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="3">
+      <c r="W3" s="3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="20">
         <v>0</v>
       </c>
       <c r="AE3" s="3">
@@ -1225,46 +1215,50 @@
       <c r="AI3" s="3">
         <v>0</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AJ3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AL3" s="5">
         <v>0.51026231569116942</v>
       </c>
-      <c r="AL3" s="5" t="s">
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="6">
+      <c r="AR3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="6">
         <v>2.8174999999999999</v>
       </c>
-      <c r="AR3" s="8">
+      <c r="AT3" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="8">
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="8">
         <v>0.95636867792127611</v>
       </c>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
       <c r="AW3" s="8"/>
       <c r="AX3" s="8"/>
-      <c r="AY3" s="3" t="s">
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>615</v>
       </c>
@@ -1299,45 +1293,45 @@
       <c r="P4" s="18">
         <v>2</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S4" s="3" t="str">
+      <c r="T4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_46_cc</v>
       </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
+      <c r="U4" s="3"/>
       <c r="V4" s="3">
         <v>0</v>
       </c>
-      <c r="W4" s="16">
-        <v>0</v>
-      </c>
-      <c r="X4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="3">
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="20">
         <v>0</v>
       </c>
       <c r="AE4" s="3">
@@ -1355,44 +1349,48 @@
       <c r="AI4" s="3">
         <v>0</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AJ4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AK4" s="5">
+      <c r="AL4" s="5">
         <v>0.45438760079739932</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="6">
+      <c r="AR4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="6">
         <v>2.5374999999999996</v>
       </c>
-      <c r="AR4" s="8">
+      <c r="AT4" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="8">
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="8">
         <v>0.86132582794152224</v>
       </c>
-      <c r="AU4" s="8"/>
-      <c r="AV4" s="8"/>
       <c r="AW4" s="8"/>
       <c r="AX4" s="8"/>
-      <c r="AY4" s="3"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="3"/>
     </row>
-    <row r="5" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>616</v>
       </c>
@@ -1425,43 +1423,43 @@
       <c r="P5" s="18">
         <v>2</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="3" t="s">
+      <c r="Q5" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="3" t="str">
+      <c r="T5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
+      <c r="U5" s="3"/>
       <c r="V5" s="3">
         <v>0</v>
       </c>
-      <c r="W5" s="16">
-        <v>0</v>
-      </c>
-      <c r="X5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="3">
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="20">
         <v>0</v>
       </c>
       <c r="AE5" s="3">
@@ -1479,44 +1477,48 @@
       <c r="AI5" s="3">
         <v>0</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AJ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AK5" s="5">
+      <c r="AL5" s="5">
         <v>0.495843034428261</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM5" s="3" t="s">
+      <c r="AO5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN5" s="3" t="s">
+      <c r="AP5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO5" s="3" t="s">
+      <c r="AQ5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="6">
+      <c r="AR5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="6">
         <v>2.6975000000000002</v>
       </c>
-      <c r="AR5" s="8">
+      <c r="AT5" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="8">
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="8">
         <v>0.91563602792995336</v>
       </c>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8"/>
       <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
-      <c r="AY5" s="3"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BA5" s="3"/>
     </row>
-    <row r="6" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>617</v>
       </c>
@@ -1547,45 +1549,45 @@
       <c r="P6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="3" t="str">
+      <c r="T6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
+      <c r="U6" s="3"/>
       <c r="V6" s="3">
         <v>0</v>
       </c>
-      <c r="W6" s="16">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="3">
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="20">
         <v>0</v>
       </c>
       <c r="AE6" s="3">
@@ -1603,44 +1605,48 @@
       <c r="AI6" s="3">
         <v>0</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AJ6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AL6" s="5">
         <v>0.45438760079739932</v>
       </c>
-      <c r="AL6" s="5" t="s">
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM6" s="3" t="s">
+      <c r="AO6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN6" s="3" t="s">
+      <c r="AP6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO6" s="3" t="s">
+      <c r="AQ6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="6">
+      <c r="AR6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="6">
         <v>2.8974999999999991</v>
       </c>
-      <c r="AR6" s="8">
+      <c r="AT6" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="8">
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="8">
         <v>0.98347485400488432</v>
       </c>
-      <c r="AU6" s="8"/>
-      <c r="AV6" s="8"/>
       <c r="AW6" s="8"/>
       <c r="AX6" s="8"/>
-      <c r="AY6" s="3"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="3"/>
     </row>
-    <row r="7" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>618</v>
       </c>
@@ -1671,43 +1677,43 @@
       <c r="P7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="3" t="s">
+      <c r="Q7" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="4"/>
+      <c r="S7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="3" t="str">
+      <c r="T7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
+      <c r="U7" s="3"/>
       <c r="V7" s="3">
         <v>0</v>
       </c>
-      <c r="W7" s="16">
-        <v>0</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="3">
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="20">
         <v>0</v>
       </c>
       <c r="AE7" s="3">
@@ -1725,44 +1731,48 @@
       <c r="AI7" s="3">
         <v>0</v>
       </c>
-      <c r="AJ7" s="4" t="s">
+      <c r="AJ7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AL7" s="5">
         <v>0.44717796016594541</v>
       </c>
-      <c r="AL7" s="5" t="s">
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM7" s="3" t="s">
+      <c r="AO7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN7" s="3" t="s">
+      <c r="AP7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO7" s="3" t="s">
+      <c r="AQ7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ7" s="6">
+      <c r="AR7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="6">
         <v>2.7875000000000001</v>
       </c>
-      <c r="AR7" s="8">
+      <c r="AT7" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="8">
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="8">
         <v>0.94613844884852993</v>
       </c>
-      <c r="AU7" s="8"/>
-      <c r="AV7" s="8"/>
       <c r="AW7" s="8"/>
       <c r="AX7" s="8"/>
-      <c r="AY7" s="3"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BA7" s="3"/>
     </row>
-    <row r="8" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>619</v>
       </c>
@@ -1793,43 +1803,43 @@
       <c r="P8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="3" t="s">
+      <c r="Q8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S8" s="3" t="str">
+      <c r="T8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
+      <c r="U8" s="3"/>
       <c r="V8" s="3">
         <v>0</v>
       </c>
-      <c r="W8" s="16">
-        <v>0</v>
-      </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="3">
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="20">
         <v>0</v>
       </c>
       <c r="AE8" s="3">
@@ -1847,44 +1857,48 @@
       <c r="AI8" s="3">
         <v>0</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AJ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AL8" s="5">
         <v>0.49223821411253404</v>
       </c>
-      <c r="AL8" s="5" t="s">
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM8" s="3" t="s">
+      <c r="AO8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN8" s="3" t="s">
+      <c r="AP8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO8" s="3" t="s">
+      <c r="AQ8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ8" s="6">
+      <c r="AR8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="6">
         <v>2.2874999999999996</v>
       </c>
-      <c r="AR8" s="8">
+      <c r="AT8" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS8" s="3"/>
-      <c r="AT8" s="8">
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="8">
         <v>0.77642751631964557</v>
       </c>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
       <c r="AW8" s="8"/>
       <c r="AX8" s="8"/>
-      <c r="AY8" s="3"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BA8" s="3"/>
     </row>
-    <row r="9" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>620</v>
       </c>
@@ -1917,45 +1931,45 @@
       <c r="P9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="3" t="str">
+      <c r="T9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
+      <c r="U9" s="3"/>
       <c r="V9" s="3">
         <v>0</v>
       </c>
-      <c r="W9" s="16">
-        <v>0</v>
-      </c>
-      <c r="X9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="3">
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="20">
         <v>0</v>
       </c>
       <c r="AE9" s="3">
@@ -1973,44 +1987,48 @@
       <c r="AI9" s="3">
         <v>0</v>
       </c>
-      <c r="AJ9" s="4" t="s">
+      <c r="AJ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AK9" s="5">
+      <c r="AL9" s="5">
         <v>0.4435731398502184</v>
       </c>
-      <c r="AL9" s="5" t="s">
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM9" s="3" t="s">
+      <c r="AO9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN9" s="3" t="s">
+      <c r="AP9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO9" s="3" t="s">
+      <c r="AQ9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ9" s="6">
+      <c r="AR9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS9" s="6">
         <v>2.4275000000000007</v>
       </c>
-      <c r="AR9" s="8">
+      <c r="AT9" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS9" s="3"/>
-      <c r="AT9" s="8">
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="8">
         <v>0.82482778469161488</v>
       </c>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
       <c r="AW9" s="8"/>
       <c r="AX9" s="8"/>
-      <c r="AY9" s="3"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
+      <c r="BA9" s="3"/>
     </row>
-    <row r="10" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>621</v>
       </c>
@@ -2041,43 +2059,43 @@
       <c r="P10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="3" t="s">
+      <c r="Q10" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S10" s="3" t="str">
+      <c r="T10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3">
-        <v>0</v>
-      </c>
+      <c r="U10" s="3"/>
       <c r="V10" s="3">
         <v>0</v>
       </c>
-      <c r="W10" s="16">
-        <v>0</v>
-      </c>
-      <c r="X10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="3">
+      <c r="W10" s="3">
+        <v>0</v>
+      </c>
+      <c r="X10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="20">
         <v>0</v>
       </c>
       <c r="AE10" s="3">
@@ -2095,44 +2113,48 @@
       <c r="AI10" s="3">
         <v>0</v>
       </c>
-      <c r="AJ10" s="4" t="s">
+      <c r="AJ10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AK10" s="5">
+      <c r="AL10" s="5">
         <v>0.46796696177456504</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM10" s="3" t="s">
+      <c r="AO10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN10" s="3" t="s">
+      <c r="AP10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO10" s="3" t="s">
+      <c r="AQ10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ10" s="6">
+      <c r="AR10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS10" s="6">
         <v>2.5474999999999994</v>
       </c>
-      <c r="AR10" s="8">
+      <c r="AT10" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="8">
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="8">
         <v>0.86560196972271386</v>
       </c>
-      <c r="AU10" s="8"/>
-      <c r="AV10" s="8"/>
       <c r="AW10" s="8"/>
       <c r="AX10" s="8"/>
-      <c r="AY10" s="3"/>
+      <c r="AY10" s="8"/>
+      <c r="AZ10" s="8"/>
+      <c r="BA10" s="3"/>
     </row>
-    <row r="11" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>622</v>
       </c>
@@ -2163,43 +2185,43 @@
       <c r="P11" s="18">
         <v>1</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="3" t="s">
+      <c r="Q11" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="3" t="str">
+      <c r="T11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
+      <c r="U11" s="3"/>
       <c r="V11" s="3">
         <v>0</v>
       </c>
-      <c r="W11" s="16">
-        <v>0</v>
-      </c>
-      <c r="X11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="3">
+      <c r="W11" s="3">
+        <v>0</v>
+      </c>
+      <c r="X11" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="20">
         <v>0</v>
       </c>
       <c r="AE11" s="3">
@@ -2217,44 +2239,48 @@
       <c r="AI11" s="3">
         <v>0</v>
       </c>
-      <c r="AJ11" s="4" t="s">
+      <c r="AJ11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK11" s="5">
+      <c r="AL11" s="5">
         <v>0.48595800259460387</v>
       </c>
-      <c r="AL11" s="5" t="s">
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM11" s="3" t="s">
+      <c r="AO11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN11" s="3" t="s">
+      <c r="AP11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO11" s="3" t="s">
+      <c r="AQ11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ11" s="6">
+      <c r="AR11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="6">
         <v>2.8974999999999991</v>
       </c>
-      <c r="AR11" s="8">
+      <c r="AT11" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS11" s="3"/>
-      <c r="AT11" s="8">
+      <c r="AU11" s="3"/>
+      <c r="AV11" s="8">
         <v>0.98391075898148517</v>
       </c>
-      <c r="AU11" s="8"/>
-      <c r="AV11" s="8"/>
       <c r="AW11" s="8"/>
       <c r="AX11" s="8"/>
-      <c r="AY11" s="3"/>
+      <c r="AY11" s="8"/>
+      <c r="AZ11" s="8"/>
+      <c r="BA11" s="3"/>
     </row>
-    <row r="12" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>623</v>
       </c>
@@ -2285,43 +2311,43 @@
       <c r="P12" s="18">
         <v>1</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="3" t="s">
+      <c r="Q12" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S12" s="3" t="str">
+      <c r="T12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3">
-        <v>0</v>
-      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3">
         <v>0</v>
       </c>
-      <c r="W12" s="16">
-        <v>0</v>
-      </c>
-      <c r="X12" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="3">
+      <c r="W12" s="3">
+        <v>0</v>
+      </c>
+      <c r="X12" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="20">
         <v>0</v>
       </c>
       <c r="AE12" s="3">
@@ -2339,44 +2365,48 @@
       <c r="AI12" s="3">
         <v>0</v>
       </c>
-      <c r="AJ12" s="4" t="s">
+      <c r="AJ12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AK12" s="5">
+      <c r="AL12" s="5">
         <v>0.55592316133919994</v>
       </c>
-      <c r="AL12" s="5" t="s">
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM12" s="3" t="s">
+      <c r="AO12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN12" s="3" t="s">
+      <c r="AP12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO12" s="3" t="s">
+      <c r="AQ12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="6">
+      <c r="AR12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="6">
         <v>2.9074999999999984</v>
       </c>
-      <c r="AR12" s="8">
+      <c r="AT12" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="8">
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="8">
         <v>0.98730648204958338</v>
       </c>
-      <c r="AU12" s="8"/>
-      <c r="AV12" s="8"/>
       <c r="AW12" s="8"/>
       <c r="AX12" s="8"/>
-      <c r="AY12" s="3"/>
+      <c r="AY12" s="8"/>
+      <c r="AZ12" s="8"/>
+      <c r="BA12" s="3"/>
     </row>
-    <row r="13" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>624</v>
       </c>
@@ -2407,43 +2437,43 @@
       <c r="P13" s="18">
         <v>1</v>
       </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="3" t="s">
+      <c r="Q13" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R13" s="4"/>
+      <c r="S13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S13" s="3" t="str">
+      <c r="T13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3">
-        <v>0</v>
-      </c>
+      <c r="U13" s="3"/>
       <c r="V13" s="3">
         <v>0</v>
       </c>
-      <c r="W13" s="16">
-        <v>0</v>
-      </c>
-      <c r="X13" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="3">
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="20">
         <v>0</v>
       </c>
       <c r="AE13" s="3">
@@ -2461,44 +2491,48 @@
       <c r="AI13" s="3">
         <v>0</v>
       </c>
-      <c r="AJ13" s="4" t="s">
+      <c r="AJ13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AK13" s="5">
+      <c r="AL13" s="5">
         <v>0.64188035636827412</v>
       </c>
-      <c r="AL13" s="5" t="s">
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM13" s="3" t="s">
+      <c r="AO13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN13" s="3" t="s">
+      <c r="AP13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO13" s="3" t="s">
+      <c r="AQ13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="6">
+      <c r="AR13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="6">
         <v>2.817499999999999</v>
       </c>
-      <c r="AR13" s="8">
+      <c r="AT13" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS13" s="3"/>
-      <c r="AT13" s="8">
+      <c r="AU13" s="3"/>
+      <c r="AV13" s="8">
         <v>0.95705764295167428</v>
       </c>
-      <c r="AU13" s="8"/>
-      <c r="AV13" s="8"/>
       <c r="AW13" s="8"/>
       <c r="AX13" s="8"/>
-      <c r="AY13" s="3"/>
+      <c r="AY13" s="8"/>
+      <c r="AZ13" s="8"/>
+      <c r="BA13" s="3"/>
     </row>
-    <row r="14" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>625</v>
       </c>
@@ -2529,43 +2563,43 @@
       <c r="P14" s="18">
         <v>1</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="3" t="s">
+      <c r="Q14" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="4"/>
+      <c r="S14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="3" t="str">
+      <c r="T14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3">
-        <v>0</v>
-      </c>
+      <c r="U14" s="3"/>
       <c r="V14" s="3">
         <v>0</v>
       </c>
-      <c r="W14" s="16">
-        <v>0</v>
-      </c>
-      <c r="X14" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="3">
+      <c r="W14" s="3">
+        <v>0</v>
+      </c>
+      <c r="X14" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="20">
         <v>0</v>
       </c>
       <c r="AE14" s="3">
@@ -2583,44 +2617,48 @@
       <c r="AI14" s="3">
         <v>0</v>
       </c>
-      <c r="AJ14" s="4" t="s">
+      <c r="AJ14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AK14" s="5">
+      <c r="AL14" s="5">
         <v>0.4799609889879245</v>
       </c>
-      <c r="AL14" s="5" t="s">
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM14" s="3" t="s">
+      <c r="AO14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN14" s="3" t="s">
+      <c r="AP14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO14" s="3" t="s">
+      <c r="AQ14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ14" s="6">
+      <c r="AR14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="6">
         <v>2.3974999999999986</v>
       </c>
-      <c r="AR14" s="8">
+      <c r="AT14" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS14" s="3"/>
-      <c r="AT14" s="8">
+      <c r="AU14" s="3"/>
+      <c r="AV14" s="8">
         <v>0.81412460557656952</v>
       </c>
-      <c r="AU14" s="8"/>
-      <c r="AV14" s="8"/>
       <c r="AW14" s="8"/>
       <c r="AX14" s="8"/>
-      <c r="AY14" s="3"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
+      <c r="BA14" s="3"/>
     </row>
-    <row r="15" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>626</v>
       </c>
@@ -2651,43 +2689,43 @@
       <c r="P15" s="18">
         <v>1</v>
       </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="3" t="s">
+      <c r="Q15" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R15" s="4"/>
+      <c r="S15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S15" s="3" t="str">
+      <c r="T15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3">
-        <v>0</v>
-      </c>
+      <c r="U15" s="3"/>
       <c r="V15" s="3">
         <v>0</v>
       </c>
-      <c r="W15" s="16">
-        <v>0</v>
-      </c>
-      <c r="X15" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="3">
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="20">
         <v>0</v>
       </c>
       <c r="AE15" s="3">
@@ -2705,44 +2743,48 @@
       <c r="AI15" s="3">
         <v>0</v>
       </c>
-      <c r="AJ15" s="4" t="s">
+      <c r="AJ15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AK15" s="5">
+      <c r="AL15" s="5">
         <v>0.48995601166572411</v>
       </c>
-      <c r="AL15" s="5" t="s">
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM15" s="3" t="s">
+      <c r="AO15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN15" s="3" t="s">
+      <c r="AP15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO15" s="3" t="s">
+      <c r="AQ15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ15" s="6">
+      <c r="AR15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS15" s="6">
         <v>2.8274999999999983</v>
       </c>
-      <c r="AR15" s="8">
+      <c r="AT15" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS15" s="3"/>
-      <c r="AT15" s="8">
+      <c r="AU15" s="3"/>
+      <c r="AV15" s="8">
         <v>0.96014069750479669</v>
       </c>
-      <c r="AU15" s="8"/>
-      <c r="AV15" s="8"/>
       <c r="AW15" s="8"/>
       <c r="AX15" s="8"/>
-      <c r="AY15" s="3"/>
+      <c r="AY15" s="8"/>
+      <c r="AZ15" s="8"/>
+      <c r="BA15" s="3"/>
     </row>
-    <row r="16" spans="1:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>627</v>
       </c>
@@ -2775,43 +2817,43 @@
       <c r="P16" s="18">
         <v>1</v>
       </c>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="3" t="s">
+      <c r="Q16" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R16" s="4"/>
+      <c r="S16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S16" s="3" t="str">
+      <c r="T16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>20160805_test001_47_cc</v>
       </c>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3">
-        <v>0</v>
-      </c>
+      <c r="U16" s="3"/>
       <c r="V16" s="3">
         <v>0</v>
       </c>
-      <c r="W16" s="16">
-        <v>0</v>
-      </c>
-      <c r="X16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="3">
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="20">
         <v>0</v>
       </c>
       <c r="AE16" s="3">
@@ -2829,44 +2871,48 @@
       <c r="AI16" s="3">
         <v>0</v>
       </c>
-      <c r="AJ16" s="4" t="s">
+      <c r="AJ16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" s="5">
+      <c r="AL16" s="5">
         <v>0.52993610237692124</v>
       </c>
-      <c r="AL16" s="5" t="s">
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM16" s="3" t="s">
+      <c r="AO16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN16" s="3" t="s">
+      <c r="AP16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO16" s="3" t="s">
+      <c r="AQ16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ16" s="6">
+      <c r="AR16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="6">
         <v>5.1874999999999991</v>
       </c>
-      <c r="AR16" s="8">
+      <c r="AT16" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS16" s="3"/>
-      <c r="AT16" s="8">
+      <c r="AU16" s="3"/>
+      <c r="AV16" s="8">
         <v>1.7621070178568985</v>
       </c>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
       <c r="AW16" s="8"/>
       <c r="AX16" s="8"/>
-      <c r="AY16" s="3"/>
+      <c r="AY16" s="8"/>
+      <c r="AZ16" s="8"/>
+      <c r="BA16" s="3"/>
     </row>
-    <row r="17" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>628</v>
       </c>
@@ -2888,42 +2934,42 @@
       <c r="P17" s="19">
         <v>1</v>
       </c>
-      <c r="R17" s="3" t="s">
+      <c r="Q17" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="S17" s="3" t="str">
-        <f t="shared" ref="S17:S19" si="1">R17</f>
+      <c r="T17" s="3" t="str">
+        <f t="shared" ref="T17:T19" si="1">S17</f>
         <v>maccor_001</v>
       </c>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3">
-        <v>0</v>
-      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3">
         <v>0</v>
       </c>
-      <c r="W17" s="16">
-        <v>0</v>
-      </c>
-      <c r="X17" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="3">
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="20">
         <v>0</v>
       </c>
       <c r="AE17" s="3">
@@ -2941,44 +2987,48 @@
       <c r="AI17" s="3">
         <v>0</v>
       </c>
-      <c r="AJ17" s="4" t="s">
+      <c r="AJ17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK17" s="5">
+      <c r="AL17" s="5">
         <v>0.52993610237692124</v>
       </c>
-      <c r="AL17" s="5" t="s">
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM17" s="3" t="s">
+      <c r="AO17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN17" s="3" t="s">
+      <c r="AP17" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO17" s="3" t="s">
+      <c r="AQ17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ17" s="6">
+      <c r="AR17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS17" s="6">
         <v>5.1874999999999991</v>
       </c>
-      <c r="AR17" s="8">
+      <c r="AT17" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS17" s="3"/>
-      <c r="AT17" s="8">
+      <c r="AU17" s="3"/>
+      <c r="AV17" s="8">
         <v>1.7621070178568985</v>
       </c>
-      <c r="AU17" s="8"/>
-      <c r="AV17" s="8"/>
       <c r="AW17" s="8"/>
       <c r="AX17" s="8"/>
-      <c r="AY17" s="3"/>
+      <c r="AY17" s="8"/>
+      <c r="AZ17" s="8"/>
+      <c r="BA17" s="3"/>
     </row>
-    <row r="18" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>629</v>
       </c>
@@ -3000,42 +3050,42 @@
       <c r="P18" s="19">
         <v>1</v>
       </c>
-      <c r="R18" s="3" t="s">
+      <c r="Q18" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="S18" s="3" t="str">
+      <c r="T18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>custom_data_001</v>
       </c>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3">
-        <v>0</v>
-      </c>
+      <c r="U18" s="3"/>
       <c r="V18" s="3">
         <v>0</v>
       </c>
-      <c r="W18" s="16">
-        <v>0</v>
-      </c>
-      <c r="X18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="3">
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="20">
         <v>0</v>
       </c>
       <c r="AE18" s="3">
@@ -3053,44 +3103,48 @@
       <c r="AI18" s="3">
         <v>0</v>
       </c>
-      <c r="AJ18" s="4" t="s">
+      <c r="AJ18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK18" s="5">
+      <c r="AL18" s="5">
         <v>0.52993610237692124</v>
       </c>
-      <c r="AL18" s="5" t="s">
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM18" s="3" t="s">
+      <c r="AO18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN18" s="3" t="s">
+      <c r="AP18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AO18" s="3" t="s">
+      <c r="AQ18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ18" s="6">
+      <c r="AR18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS18" s="6">
         <v>5.1874999999999991</v>
       </c>
-      <c r="AR18" s="8">
+      <c r="AT18" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS18" s="3"/>
-      <c r="AT18" s="8">
+      <c r="AU18" s="3"/>
+      <c r="AV18" s="8">
         <v>1.7621070178568985</v>
       </c>
-      <c r="AU18" s="8"/>
-      <c r="AV18" s="8"/>
       <c r="AW18" s="8"/>
       <c r="AX18" s="8"/>
-      <c r="AY18" s="3"/>
+      <c r="AY18" s="8"/>
+      <c r="AZ18" s="8"/>
+      <c r="BA18" s="3"/>
     </row>
-    <row r="19" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>630</v>
       </c>
@@ -3112,42 +3166,42 @@
       <c r="P19" s="19">
         <v>1</v>
       </c>
-      <c r="R19" s="3" t="s">
+      <c r="Q19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S19" s="3" t="str">
+      <c r="T19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>custom_data_002</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3">
-        <v>0</v>
-      </c>
+      <c r="U19" s="3"/>
       <c r="V19" s="3">
         <v>0</v>
       </c>
-      <c r="W19" s="16">
-        <v>0</v>
-      </c>
-      <c r="X19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="12">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="3">
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="20">
         <v>0</v>
       </c>
       <c r="AE19" s="3">
@@ -3165,45 +3219,49 @@
       <c r="AI19" s="3">
         <v>0</v>
       </c>
-      <c r="AJ19" s="4" t="s">
+      <c r="AJ19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK19" s="5">
+      <c r="AL19" s="5">
         <v>0.52993610237692124</v>
       </c>
-      <c r="AL19" s="5" t="s">
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AM19" s="3" t="s">
+      <c r="AO19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AN19" s="3" t="s">
+      <c r="AP19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AO19" s="3" t="s">
+      <c r="AQ19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AP19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ19" s="6">
+      <c r="AR19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS19" s="6">
         <v>5.1874999999999991</v>
       </c>
-      <c r="AR19" s="8">
+      <c r="AT19" s="8">
         <v>1.77</v>
       </c>
-      <c r="AS19" s="3"/>
-      <c r="AT19" s="8">
+      <c r="AU19" s="3"/>
+      <c r="AV19" s="8">
         <v>1.7621070178568985</v>
       </c>
-      <c r="AU19" s="8"/>
-      <c r="AV19" s="8"/>
       <c r="AW19" s="8"/>
       <c r="AX19" s="8"/>
-      <c r="AY19" s="3"/>
+      <c r="AY19" s="8"/>
+      <c r="AZ19" s="8"/>
+      <c r="BA19" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BB16" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:BD16" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>